<commit_message>
Guide folder aangemaakt in tryouts
Guide folder aangemaakt zodat ik er later direct mee bezig kan
</commit_message>
<xml_diff>
--- a/doc/Andalusier documenten/Individuele taakverdeling/Maaike/Maaike taken.xlsx
+++ b/doc/Andalusier documenten/Individuele taakverdeling/Maaike/Maaike taken.xlsx
@@ -744,7 +744,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -993,7 +993,7 @@
       <c r="F19" s="5"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="1"/>
@@ -1007,7 +1007,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="29" t="s">
         <v>30</v>
       </c>
       <c r="B21" s="1"/>

</xml_diff>